<commit_message>
Switched from .pickle to .pkl
</commit_message>
<xml_diff>
--- a/data/xlsx/unprecedented.xlsx
+++ b/data/xlsx/unprecedented.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repositories\notebooks\covid19\data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d4b546f3686e4e1/Documents/GitHub/covid19/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BA4F63-EFA3-4098-80AC-3D8E37A26D81}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{82BA4F63-EFA3-4098-80AC-3D8E37A26D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F51576CC-5BD5-4644-B255-2ED21892A567}"/>
   <bookViews>
-    <workbookView xWindow="-18390" yWindow="-2805" windowWidth="18510" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="multiTimeline" sheetId="1" r:id="rId1"/>
+    <sheet name="by_week" sheetId="1" r:id="rId1"/>
+    <sheet name="by_month" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="252">
   <si>
     <t>Donald Trump election</t>
   </si>
@@ -83,6 +84,699 @@
   </si>
   <si>
     <t>week_topic</t>
+  </si>
+  <si>
+    <t>2022-03</t>
+  </si>
+  <si>
+    <t>2022-02</t>
+  </si>
+  <si>
+    <t>2022-01</t>
+  </si>
+  <si>
+    <t>2021-12</t>
+  </si>
+  <si>
+    <t>2021-11</t>
+  </si>
+  <si>
+    <t>2021-10</t>
+  </si>
+  <si>
+    <t>2021-09</t>
+  </si>
+  <si>
+    <t>2021-08</t>
+  </si>
+  <si>
+    <t>2021-07</t>
+  </si>
+  <si>
+    <t>2021-06</t>
+  </si>
+  <si>
+    <t>2021-05</t>
+  </si>
+  <si>
+    <t>2021-04</t>
+  </si>
+  <si>
+    <t>2021-03</t>
+  </si>
+  <si>
+    <t>2021-02</t>
+  </si>
+  <si>
+    <t>2021-01</t>
+  </si>
+  <si>
+    <t>2020-12</t>
+  </si>
+  <si>
+    <t>2020-11</t>
+  </si>
+  <si>
+    <t>2020-10</t>
+  </si>
+  <si>
+    <t>2020-09</t>
+  </si>
+  <si>
+    <t>2020-08</t>
+  </si>
+  <si>
+    <t>2020-07</t>
+  </si>
+  <si>
+    <t>2020-06</t>
+  </si>
+  <si>
+    <t>2020-05</t>
+  </si>
+  <si>
+    <t>2020-04</t>
+  </si>
+  <si>
+    <t>2020-03</t>
+  </si>
+  <si>
+    <t>2020-02</t>
+  </si>
+  <si>
+    <t>2020-01</t>
+  </si>
+  <si>
+    <t>2019-12</t>
+  </si>
+  <si>
+    <t>2019-11</t>
+  </si>
+  <si>
+    <t>2019-10</t>
+  </si>
+  <si>
+    <t>2019-09</t>
+  </si>
+  <si>
+    <t>2019-08</t>
+  </si>
+  <si>
+    <t>2019-07</t>
+  </si>
+  <si>
+    <t>2019-06</t>
+  </si>
+  <si>
+    <t>2019-05</t>
+  </si>
+  <si>
+    <t>2019-04</t>
+  </si>
+  <si>
+    <t>2019-03</t>
+  </si>
+  <si>
+    <t>2019-02</t>
+  </si>
+  <si>
+    <t>2019-01</t>
+  </si>
+  <si>
+    <t>2018-12</t>
+  </si>
+  <si>
+    <t>2018-11</t>
+  </si>
+  <si>
+    <t>2018-10</t>
+  </si>
+  <si>
+    <t>2018-09</t>
+  </si>
+  <si>
+    <t>2018-08</t>
+  </si>
+  <si>
+    <t>2018-07</t>
+  </si>
+  <si>
+    <t>2018-06</t>
+  </si>
+  <si>
+    <t>2018-05</t>
+  </si>
+  <si>
+    <t>2018-04</t>
+  </si>
+  <si>
+    <t>2018-03</t>
+  </si>
+  <si>
+    <t>2018-02</t>
+  </si>
+  <si>
+    <t>2018-01</t>
+  </si>
+  <si>
+    <t>2017-12</t>
+  </si>
+  <si>
+    <t>2017-11</t>
+  </si>
+  <si>
+    <t>2017-10</t>
+  </si>
+  <si>
+    <t>2017-09</t>
+  </si>
+  <si>
+    <t>2017-08</t>
+  </si>
+  <si>
+    <t>2017-07</t>
+  </si>
+  <si>
+    <t>2017-06</t>
+  </si>
+  <si>
+    <t>2017-05</t>
+  </si>
+  <si>
+    <t>2017-04</t>
+  </si>
+  <si>
+    <t>2017-03</t>
+  </si>
+  <si>
+    <t>2017-02</t>
+  </si>
+  <si>
+    <t>2017-01</t>
+  </si>
+  <si>
+    <t>2016-12</t>
+  </si>
+  <si>
+    <t>2016-11</t>
+  </si>
+  <si>
+    <t>2016-10</t>
+  </si>
+  <si>
+    <t>2016-09</t>
+  </si>
+  <si>
+    <t>2016-08</t>
+  </si>
+  <si>
+    <t>2016-07</t>
+  </si>
+  <si>
+    <t>2016-06</t>
+  </si>
+  <si>
+    <t>2016-05</t>
+  </si>
+  <si>
+    <t>2016-04</t>
+  </si>
+  <si>
+    <t>2016-03</t>
+  </si>
+  <si>
+    <t>2016-02</t>
+  </si>
+  <si>
+    <t>2016-01</t>
+  </si>
+  <si>
+    <t>2015-12</t>
+  </si>
+  <si>
+    <t>2015-11</t>
+  </si>
+  <si>
+    <t>2015-10</t>
+  </si>
+  <si>
+    <t>2015-09</t>
+  </si>
+  <si>
+    <t>2015-08</t>
+  </si>
+  <si>
+    <t>2015-07</t>
+  </si>
+  <si>
+    <t>2015-06</t>
+  </si>
+  <si>
+    <t>2015-05</t>
+  </si>
+  <si>
+    <t>2015-04</t>
+  </si>
+  <si>
+    <t>2015-03</t>
+  </si>
+  <si>
+    <t>2015-02</t>
+  </si>
+  <si>
+    <t>2015-01</t>
+  </si>
+  <si>
+    <t>2014-12</t>
+  </si>
+  <si>
+    <t>2014-11</t>
+  </si>
+  <si>
+    <t>2014-10</t>
+  </si>
+  <si>
+    <t>2014-09</t>
+  </si>
+  <si>
+    <t>2014-08</t>
+  </si>
+  <si>
+    <t>2014-07</t>
+  </si>
+  <si>
+    <t>2014-06</t>
+  </si>
+  <si>
+    <t>2014-05</t>
+  </si>
+  <si>
+    <t>2014-04</t>
+  </si>
+  <si>
+    <t>2014-03</t>
+  </si>
+  <si>
+    <t>2014-02</t>
+  </si>
+  <si>
+    <t>2014-01</t>
+  </si>
+  <si>
+    <t>2013-12</t>
+  </si>
+  <si>
+    <t>2013-11</t>
+  </si>
+  <si>
+    <t>2013-10</t>
+  </si>
+  <si>
+    <t>2013-09</t>
+  </si>
+  <si>
+    <t>2013-08</t>
+  </si>
+  <si>
+    <t>2013-07</t>
+  </si>
+  <si>
+    <t>2013-06</t>
+  </si>
+  <si>
+    <t>2013-05</t>
+  </si>
+  <si>
+    <t>2013-04</t>
+  </si>
+  <si>
+    <t>2013-03</t>
+  </si>
+  <si>
+    <t>2013-02</t>
+  </si>
+  <si>
+    <t>2013-01</t>
+  </si>
+  <si>
+    <t>2012-12</t>
+  </si>
+  <si>
+    <t>2012-11</t>
+  </si>
+  <si>
+    <t>2012-10</t>
+  </si>
+  <si>
+    <t>2012-09</t>
+  </si>
+  <si>
+    <t>2012-08</t>
+  </si>
+  <si>
+    <t>2012-07</t>
+  </si>
+  <si>
+    <t>2012-06</t>
+  </si>
+  <si>
+    <t>2012-05</t>
+  </si>
+  <si>
+    <t>2012-04</t>
+  </si>
+  <si>
+    <t>2012-03</t>
+  </si>
+  <si>
+    <t>2012-02</t>
+  </si>
+  <si>
+    <t>2012-01</t>
+  </si>
+  <si>
+    <t>2011-12</t>
+  </si>
+  <si>
+    <t>2011-11</t>
+  </si>
+  <si>
+    <t>2011-10</t>
+  </si>
+  <si>
+    <t>2011-09</t>
+  </si>
+  <si>
+    <t>2011-08</t>
+  </si>
+  <si>
+    <t>2011-07</t>
+  </si>
+  <si>
+    <t>2011-06</t>
+  </si>
+  <si>
+    <t>2011-05</t>
+  </si>
+  <si>
+    <t>2011-04</t>
+  </si>
+  <si>
+    <t>2011-03</t>
+  </si>
+  <si>
+    <t>2011-02</t>
+  </si>
+  <si>
+    <t>2011-01</t>
+  </si>
+  <si>
+    <t>2010-12</t>
+  </si>
+  <si>
+    <t>2010-11</t>
+  </si>
+  <si>
+    <t>2010-10</t>
+  </si>
+  <si>
+    <t>2010-09</t>
+  </si>
+  <si>
+    <t>2010-08</t>
+  </si>
+  <si>
+    <t>2010-07</t>
+  </si>
+  <si>
+    <t>2010-06</t>
+  </si>
+  <si>
+    <t>2010-05</t>
+  </si>
+  <si>
+    <t>2010-04</t>
+  </si>
+  <si>
+    <t>2010-03</t>
+  </si>
+  <si>
+    <t>2010-02</t>
+  </si>
+  <si>
+    <t>2010-01</t>
+  </si>
+  <si>
+    <t>2009-12</t>
+  </si>
+  <si>
+    <t>2009-11</t>
+  </si>
+  <si>
+    <t>2009-10</t>
+  </si>
+  <si>
+    <t>2009-09</t>
+  </si>
+  <si>
+    <t>2009-08</t>
+  </si>
+  <si>
+    <t>2009-07</t>
+  </si>
+  <si>
+    <t>2009-06</t>
+  </si>
+  <si>
+    <t>2009-05</t>
+  </si>
+  <si>
+    <t>2009-04</t>
+  </si>
+  <si>
+    <t>2009-03</t>
+  </si>
+  <si>
+    <t>2009-02</t>
+  </si>
+  <si>
+    <t>2009-01</t>
+  </si>
+  <si>
+    <t>2008-12</t>
+  </si>
+  <si>
+    <t>2008-11</t>
+  </si>
+  <si>
+    <t>2008-10</t>
+  </si>
+  <si>
+    <t>2008-09</t>
+  </si>
+  <si>
+    <t>2008-08</t>
+  </si>
+  <si>
+    <t>2008-07</t>
+  </si>
+  <si>
+    <t>2008-06</t>
+  </si>
+  <si>
+    <t>2008-05</t>
+  </si>
+  <si>
+    <t>2008-04</t>
+  </si>
+  <si>
+    <t>2008-03</t>
+  </si>
+  <si>
+    <t>2008-02</t>
+  </si>
+  <si>
+    <t>2008-01</t>
+  </si>
+  <si>
+    <t>2007-12</t>
+  </si>
+  <si>
+    <t>2007-11</t>
+  </si>
+  <si>
+    <t>2007-10</t>
+  </si>
+  <si>
+    <t>2007-09</t>
+  </si>
+  <si>
+    <t>2007-08</t>
+  </si>
+  <si>
+    <t>2007-07</t>
+  </si>
+  <si>
+    <t>2007-06</t>
+  </si>
+  <si>
+    <t>2007-05</t>
+  </si>
+  <si>
+    <t>2007-04</t>
+  </si>
+  <si>
+    <t>2007-03</t>
+  </si>
+  <si>
+    <t>2007-02</t>
+  </si>
+  <si>
+    <t>2007-01</t>
+  </si>
+  <si>
+    <t>2006-12</t>
+  </si>
+  <si>
+    <t>2006-11</t>
+  </si>
+  <si>
+    <t>2006-10</t>
+  </si>
+  <si>
+    <t>2006-09</t>
+  </si>
+  <si>
+    <t>2006-08</t>
+  </si>
+  <si>
+    <t>2006-07</t>
+  </si>
+  <si>
+    <t>2006-06</t>
+  </si>
+  <si>
+    <t>2006-05</t>
+  </si>
+  <si>
+    <t>2006-04</t>
+  </si>
+  <si>
+    <t>2006-03</t>
+  </si>
+  <si>
+    <t>2006-02</t>
+  </si>
+  <si>
+    <t>2006-01</t>
+  </si>
+  <si>
+    <t>2005-12</t>
+  </si>
+  <si>
+    <t>2005-11</t>
+  </si>
+  <si>
+    <t>2005-10</t>
+  </si>
+  <si>
+    <t>2005-09</t>
+  </si>
+  <si>
+    <t>2005-08</t>
+  </si>
+  <si>
+    <t>2005-07</t>
+  </si>
+  <si>
+    <t>2005-06</t>
+  </si>
+  <si>
+    <t>2005-05</t>
+  </si>
+  <si>
+    <t>2005-04</t>
+  </si>
+  <si>
+    <t>2005-03</t>
+  </si>
+  <si>
+    <t>2005-02</t>
+  </si>
+  <si>
+    <t>2005-01</t>
+  </si>
+  <si>
+    <t>2004-12</t>
+  </si>
+  <si>
+    <t>2004-11</t>
+  </si>
+  <si>
+    <t>2004-10</t>
+  </si>
+  <si>
+    <t>2004-09</t>
+  </si>
+  <si>
+    <t>2004-08</t>
+  </si>
+  <si>
+    <t>2004-07</t>
+  </si>
+  <si>
+    <t>2004-06</t>
+  </si>
+  <si>
+    <t>2004-05</t>
+  </si>
+  <si>
+    <t>2004-04</t>
+  </si>
+  <si>
+    <t>2004-03</t>
+  </si>
+  <si>
+    <t>2004-02</t>
+  </si>
+  <si>
+    <t>2004-01</t>
+  </si>
+  <si>
+    <t>month_date</t>
+  </si>
+  <si>
+    <t>month_topic</t>
+  </si>
+  <si>
+    <t>The unpiloted Cassini–Huygens spacecraft arrives at Saturn.</t>
+  </si>
+  <si>
+    <t>Cassini–Huygens</t>
+  </si>
+  <si>
+    <t>Water on Moon</t>
+  </si>
+  <si>
+    <t>Having analyzed the data from the LCROSS lunar impact, NASA announces that it has found a "significant" quantity of water in the Moon's Cabeus crater.</t>
+  </si>
+  <si>
+    <t>Russia suspend from the G8</t>
+  </si>
+  <si>
+    <t>During an emergency meeting, the United Kingdom, the United States, Italy, Germany, France, Japan, and Canada temporarily suspend Russia from the G8, recognizing Crimea within Ukraine's international borders and rejecting the validity of the 2014 Crimean referendum.</t>
+  </si>
+  <si>
+    <t>Russian Defence Ministry Tupolev Tu-154 crash</t>
+  </si>
+  <si>
+    <t>A Tupolev Tu-154 jetliner of the Russian Defence Ministry crashes into the Black Sea shortly after taking off from Sochi International Airport, Russia, while en route to Khmeimim Air Base, Syria.</t>
+  </si>
+  <si>
+    <t>COVID-19 pandemic</t>
+  </si>
+  <si>
+    <t>The number of confirmed cases of COVID-19 passes 2 million worldwide.</t>
   </si>
 </sst>
 </file>
@@ -608,7 +1302,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -618,6 +1312,12 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -975,19 +1675,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1001,7 +1701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>42127</v>
       </c>
@@ -1009,7 +1709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>42134</v>
       </c>
@@ -1017,7 +1717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>42141</v>
       </c>
@@ -1025,7 +1725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42148</v>
       </c>
@@ -1033,7 +1733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>42155</v>
       </c>
@@ -1041,7 +1741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>42162</v>
       </c>
@@ -1049,7 +1749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>42169</v>
       </c>
@@ -1057,7 +1757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>42176</v>
       </c>
@@ -1065,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>42183</v>
       </c>
@@ -1073,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>42190</v>
       </c>
@@ -1081,7 +1781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>42197</v>
       </c>
@@ -1089,7 +1789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>42204</v>
       </c>
@@ -1097,7 +1797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42211</v>
       </c>
@@ -1105,7 +1805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>42218</v>
       </c>
@@ -1113,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>42225</v>
       </c>
@@ -1121,7 +1821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>42232</v>
       </c>
@@ -1129,7 +1829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>42239</v>
       </c>
@@ -1137,7 +1837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>42246</v>
       </c>
@@ -1145,7 +1845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>42253</v>
       </c>
@@ -1153,7 +1853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>42260</v>
       </c>
@@ -1161,7 +1861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>42267</v>
       </c>
@@ -1169,7 +1869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>42274</v>
       </c>
@@ -1177,7 +1877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>42281</v>
       </c>
@@ -1185,7 +1885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>42288</v>
       </c>
@@ -1193,7 +1893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>42295</v>
       </c>
@@ -1201,7 +1901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>42302</v>
       </c>
@@ -1209,7 +1909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>42309</v>
       </c>
@@ -1217,7 +1917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>42316</v>
       </c>
@@ -1225,7 +1925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>42323</v>
       </c>
@@ -1233,7 +1933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>42330</v>
       </c>
@@ -1241,7 +1941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>42337</v>
       </c>
@@ -1249,7 +1949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>42344</v>
       </c>
@@ -1257,7 +1957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>42351</v>
       </c>
@@ -1265,7 +1965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>42358</v>
       </c>
@@ -1273,7 +1973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>42365</v>
       </c>
@@ -1281,7 +1981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>42372</v>
       </c>
@@ -1289,7 +1989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>42379</v>
       </c>
@@ -1297,7 +1997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>42386</v>
       </c>
@@ -1305,7 +2005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>42393</v>
       </c>
@@ -1313,7 +2013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>42400</v>
       </c>
@@ -1321,7 +2021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>42407</v>
       </c>
@@ -1329,7 +2029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42414</v>
       </c>
@@ -1337,7 +2037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42421</v>
       </c>
@@ -1345,7 +2045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>42428</v>
       </c>
@@ -1353,7 +2053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>42435</v>
       </c>
@@ -1361,7 +2061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>42442</v>
       </c>
@@ -1369,7 +2069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>42449</v>
       </c>
@@ -1377,7 +2077,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>42456</v>
       </c>
@@ -1385,7 +2085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>42463</v>
       </c>
@@ -1393,7 +2093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>42470</v>
       </c>
@@ -1401,7 +2101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>42477</v>
       </c>
@@ -1409,7 +2109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>42484</v>
       </c>
@@ -1417,7 +2117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>42491</v>
       </c>
@@ -1425,7 +2125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>42498</v>
       </c>
@@ -1433,7 +2133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>42505</v>
       </c>
@@ -1441,7 +2141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>42512</v>
       </c>
@@ -1449,7 +2149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>42519</v>
       </c>
@@ -1457,7 +2157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>42526</v>
       </c>
@@ -1465,7 +2165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>42533</v>
       </c>
@@ -1473,7 +2173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>42540</v>
       </c>
@@ -1481,7 +2181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>42547</v>
       </c>
@@ -1489,7 +2189,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>42554</v>
       </c>
@@ -1497,7 +2197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>42561</v>
       </c>
@@ -1505,7 +2205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>42568</v>
       </c>
@@ -1513,7 +2213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>42575</v>
       </c>
@@ -1521,7 +2221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>42582</v>
       </c>
@@ -1529,7 +2229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>42589</v>
       </c>
@@ -1537,7 +2237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>42596</v>
       </c>
@@ -1545,7 +2245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>42603</v>
       </c>
@@ -1553,7 +2253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>42610</v>
       </c>
@@ -1561,7 +2261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>42617</v>
       </c>
@@ -1569,7 +2269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>42624</v>
       </c>
@@ -1577,7 +2277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>42631</v>
       </c>
@@ -1585,7 +2285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>42638</v>
       </c>
@@ -1593,7 +2293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>42645</v>
       </c>
@@ -1601,7 +2301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>42652</v>
       </c>
@@ -1609,7 +2309,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>42659</v>
       </c>
@@ -1617,7 +2317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>42666</v>
       </c>
@@ -1625,7 +2325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>42673</v>
       </c>
@@ -1633,7 +2333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>42680</v>
       </c>
@@ -1647,7 +2347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>42687</v>
       </c>
@@ -1658,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>42694</v>
       </c>
@@ -1666,7 +2366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>42701</v>
       </c>
@@ -1674,7 +2374,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>42708</v>
       </c>
@@ -1682,7 +2382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>42715</v>
       </c>
@@ -1693,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>42722</v>
       </c>
@@ -1704,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>42729</v>
       </c>
@@ -1712,7 +2412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>42736</v>
       </c>
@@ -1723,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>42743</v>
       </c>
@@ -1731,7 +2431,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>42750</v>
       </c>
@@ -1739,7 +2439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>42757</v>
       </c>
@@ -1747,7 +2447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>42764</v>
       </c>
@@ -1755,7 +2455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>42771</v>
       </c>
@@ -1763,7 +2463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>42778</v>
       </c>
@@ -1771,7 +2471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>42785</v>
       </c>
@@ -1779,7 +2479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>42792</v>
       </c>
@@ -1787,7 +2487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>42799</v>
       </c>
@@ -1795,7 +2495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>42806</v>
       </c>
@@ -1803,7 +2503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>42813</v>
       </c>
@@ -1811,7 +2511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>42820</v>
       </c>
@@ -1819,7 +2519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>42827</v>
       </c>
@@ -1827,7 +2527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>42834</v>
       </c>
@@ -1835,7 +2535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>42841</v>
       </c>
@@ -1843,7 +2543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>42848</v>
       </c>
@@ -1851,7 +2551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>42855</v>
       </c>
@@ -1859,7 +2559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>42862</v>
       </c>
@@ -1867,7 +2567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>42869</v>
       </c>
@@ -1875,7 +2575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>42876</v>
       </c>
@@ -1883,7 +2583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>42883</v>
       </c>
@@ -1891,7 +2591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>42890</v>
       </c>
@@ -1899,7 +2599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>42897</v>
       </c>
@@ -1907,7 +2607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>42904</v>
       </c>
@@ -1915,7 +2615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>42911</v>
       </c>
@@ -1923,7 +2623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>42918</v>
       </c>
@@ -1931,7 +2631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>42925</v>
       </c>
@@ -1939,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>42932</v>
       </c>
@@ -1947,7 +2647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>42939</v>
       </c>
@@ -1955,7 +2655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>42946</v>
       </c>
@@ -1963,7 +2663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>42953</v>
       </c>
@@ -1971,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>42960</v>
       </c>
@@ -1979,7 +2679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>42967</v>
       </c>
@@ -1987,7 +2687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>42974</v>
       </c>
@@ -2001,7 +2701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>42981</v>
       </c>
@@ -2009,7 +2709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>42988</v>
       </c>
@@ -2017,7 +2717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>42995</v>
       </c>
@@ -2025,7 +2725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>43002</v>
       </c>
@@ -2033,7 +2733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>43009</v>
       </c>
@@ -2041,7 +2741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>43016</v>
       </c>
@@ -2049,7 +2749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>43023</v>
       </c>
@@ -2057,7 +2757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>43030</v>
       </c>
@@ -2065,7 +2765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>43037</v>
       </c>
@@ -2073,7 +2773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>43044</v>
       </c>
@@ -2081,7 +2781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>43051</v>
       </c>
@@ -2089,7 +2789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>43058</v>
       </c>
@@ -2097,7 +2797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>43065</v>
       </c>
@@ -2105,7 +2805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>43072</v>
       </c>
@@ -2113,7 +2813,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>43079</v>
       </c>
@@ -2121,7 +2821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>43086</v>
       </c>
@@ -2129,7 +2829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>43093</v>
       </c>
@@ -2137,7 +2837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>43100</v>
       </c>
@@ -2145,7 +2845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>43107</v>
       </c>
@@ -2153,7 +2853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>43114</v>
       </c>
@@ -2161,7 +2861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>43121</v>
       </c>
@@ -2169,7 +2869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>43128</v>
       </c>
@@ -2177,7 +2877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>43135</v>
       </c>
@@ -2185,7 +2885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>43142</v>
       </c>
@@ -2193,7 +2893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>43149</v>
       </c>
@@ -2201,7 +2901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>43156</v>
       </c>
@@ -2209,7 +2909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>43163</v>
       </c>
@@ -2217,7 +2917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>43170</v>
       </c>
@@ -2225,7 +2925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>43177</v>
       </c>
@@ -2233,7 +2933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>43184</v>
       </c>
@@ -2241,7 +2941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>43191</v>
       </c>
@@ -2249,7 +2949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>43198</v>
       </c>
@@ -2257,7 +2957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>43205</v>
       </c>
@@ -2265,7 +2965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>43212</v>
       </c>
@@ -2273,7 +2973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>43219</v>
       </c>
@@ -2281,7 +2981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>43226</v>
       </c>
@@ -2289,7 +2989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>43233</v>
       </c>
@@ -2297,7 +2997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>43240</v>
       </c>
@@ -2305,7 +3005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>43247</v>
       </c>
@@ -2313,7 +3013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>43254</v>
       </c>
@@ -2321,7 +3021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>43261</v>
       </c>
@@ -2329,7 +3029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>43268</v>
       </c>
@@ -2337,7 +3037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>43275</v>
       </c>
@@ -2345,7 +3045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>43282</v>
       </c>
@@ -2353,7 +3053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>43289</v>
       </c>
@@ -2361,7 +3061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>43296</v>
       </c>
@@ -2369,7 +3069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>43303</v>
       </c>
@@ -2377,7 +3077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>43310</v>
       </c>
@@ -2385,7 +3085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>43317</v>
       </c>
@@ -2393,7 +3093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>43324</v>
       </c>
@@ -2401,7 +3101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>43331</v>
       </c>
@@ -2409,7 +3109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>43338</v>
       </c>
@@ -2417,7 +3117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>43345</v>
       </c>
@@ -2425,7 +3125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>43352</v>
       </c>
@@ -2433,7 +3133,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>43359</v>
       </c>
@@ -2441,7 +3141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>43366</v>
       </c>
@@ -2449,7 +3149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>43373</v>
       </c>
@@ -2457,7 +3157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>43380</v>
       </c>
@@ -2465,7 +3165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>43387</v>
       </c>
@@ -2473,7 +3173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>43394</v>
       </c>
@@ -2481,7 +3181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>43401</v>
       </c>
@@ -2489,7 +3189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>43408</v>
       </c>
@@ -2497,7 +3197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>43415</v>
       </c>
@@ -2505,7 +3205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>43422</v>
       </c>
@@ -2513,7 +3213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>43429</v>
       </c>
@@ -2521,7 +3221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>43436</v>
       </c>
@@ -2529,7 +3229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>43443</v>
       </c>
@@ -2537,7 +3237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>43450</v>
       </c>
@@ -2545,7 +3245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>43457</v>
       </c>
@@ -2553,7 +3253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>43464</v>
       </c>
@@ -2561,7 +3261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>43471</v>
       </c>
@@ -2569,7 +3269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>43478</v>
       </c>
@@ -2577,7 +3277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>43485</v>
       </c>
@@ -2585,7 +3285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>43492</v>
       </c>
@@ -2593,7 +3293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>43499</v>
       </c>
@@ -2601,7 +3301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>43506</v>
       </c>
@@ -2609,7 +3309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>43513</v>
       </c>
@@ -2617,7 +3317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>43520</v>
       </c>
@@ -2625,7 +3325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>43527</v>
       </c>
@@ -2633,7 +3333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>43534</v>
       </c>
@@ -2641,7 +3341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>43541</v>
       </c>
@@ -2649,7 +3349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>43548</v>
       </c>
@@ -2657,7 +3357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>43555</v>
       </c>
@@ -2665,7 +3365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>43562</v>
       </c>
@@ -2673,7 +3373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>43569</v>
       </c>
@@ -2681,7 +3381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>43576</v>
       </c>
@@ -2689,7 +3389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>43583</v>
       </c>
@@ -2697,7 +3397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>43590</v>
       </c>
@@ -2705,7 +3405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>43597</v>
       </c>
@@ -2713,7 +3413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>43604</v>
       </c>
@@ -2721,7 +3421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>43611</v>
       </c>
@@ -2729,7 +3429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>43618</v>
       </c>
@@ -2737,7 +3437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>43625</v>
       </c>
@@ -2745,7 +3445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>43632</v>
       </c>
@@ -2753,7 +3453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>43639</v>
       </c>
@@ -2761,7 +3461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>43646</v>
       </c>
@@ -2769,7 +3469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>43653</v>
       </c>
@@ -2777,7 +3477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>43660</v>
       </c>
@@ -2785,7 +3485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>43667</v>
       </c>
@@ -2793,7 +3493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>43674</v>
       </c>
@@ -2801,7 +3501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>43681</v>
       </c>
@@ -2809,7 +3509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>43688</v>
       </c>
@@ -2817,7 +3517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>43695</v>
       </c>
@@ -2825,7 +3525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>43702</v>
       </c>
@@ -2833,7 +3533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>43709</v>
       </c>
@@ -2841,7 +3541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>43716</v>
       </c>
@@ -2849,7 +3549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>43723</v>
       </c>
@@ -2857,7 +3557,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>43730</v>
       </c>
@@ -2871,7 +3571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>43737</v>
       </c>
@@ -2879,7 +3579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>43744</v>
       </c>
@@ -2887,7 +3587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>43751</v>
       </c>
@@ -2895,7 +3595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>43758</v>
       </c>
@@ -2903,7 +3603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>43765</v>
       </c>
@@ -2911,7 +3611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>43772</v>
       </c>
@@ -2919,7 +3619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>43779</v>
       </c>
@@ -2927,7 +3627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>43786</v>
       </c>
@@ -2935,7 +3635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>43793</v>
       </c>
@@ -2943,7 +3643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>43800</v>
       </c>
@@ -2951,7 +3651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>43807</v>
       </c>
@@ -2959,7 +3659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>43814</v>
       </c>
@@ -2967,7 +3667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>43821</v>
       </c>
@@ -2975,7 +3675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>43828</v>
       </c>
@@ -2983,7 +3683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>43835</v>
       </c>
@@ -2991,7 +3691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>43842</v>
       </c>
@@ -2999,7 +3699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>43849</v>
       </c>
@@ -3007,7 +3707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>43856</v>
       </c>
@@ -3015,7 +3715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>43863</v>
       </c>
@@ -3023,7 +3723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>43870</v>
       </c>
@@ -3031,7 +3731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>43877</v>
       </c>
@@ -3039,7 +3739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>43884</v>
       </c>
@@ -3050,7 +3750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>43891</v>
       </c>
@@ -3058,7 +3758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>43898</v>
       </c>
@@ -3072,7 +3772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>43905</v>
       </c>
@@ -3086,7 +3786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>43912</v>
       </c>
@@ -3100,7 +3800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>43919</v>
       </c>
@@ -3114,7 +3814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>43926</v>
       </c>
@@ -3128,7 +3828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>43933</v>
       </c>
@@ -3142,7 +3842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>43940</v>
       </c>
@@ -3174,4 +3874,1821 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9030D501-C819-459D-9444-235607ABA130}">
+  <dimension ref="A1:D220"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="D198" sqref="D198"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>219</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>211</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>210</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>203</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>202</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>201</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>194</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>191</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>189</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>185</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>182</v>
+      </c>
+      <c r="B59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>181</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>178</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>177</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>175</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>174</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>173</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>172</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>171</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>170</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>169</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>167</v>
+      </c>
+      <c r="B74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>165</v>
+      </c>
+      <c r="B76">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>164</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>163</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>156</v>
+      </c>
+      <c r="B85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>155</v>
+      </c>
+      <c r="B86">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>153</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>151</v>
+      </c>
+      <c r="B90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>150</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>148</v>
+      </c>
+      <c r="B93">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>147</v>
+      </c>
+      <c r="B94">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>146</v>
+      </c>
+      <c r="B95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>145</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>143</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>141</v>
+      </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>140</v>
+      </c>
+      <c r="B101">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>139</v>
+      </c>
+      <c r="B102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>138</v>
+      </c>
+      <c r="B103">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>137</v>
+      </c>
+      <c r="B104">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>136</v>
+      </c>
+      <c r="B105">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>135</v>
+      </c>
+      <c r="B106">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>134</v>
+      </c>
+      <c r="B107">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>133</v>
+      </c>
+      <c r="B108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>132</v>
+      </c>
+      <c r="B109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>131</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>130</v>
+      </c>
+      <c r="B111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>129</v>
+      </c>
+      <c r="B112">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>128</v>
+      </c>
+      <c r="B113">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>127</v>
+      </c>
+      <c r="B114">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>125</v>
+      </c>
+      <c r="B116">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>124</v>
+      </c>
+      <c r="B117">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>123</v>
+      </c>
+      <c r="B118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>122</v>
+      </c>
+      <c r="B119">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>119</v>
+      </c>
+      <c r="B122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>118</v>
+      </c>
+      <c r="B123">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>117</v>
+      </c>
+      <c r="B124">
+        <v>15</v>
+      </c>
+      <c r="C124" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>116</v>
+      </c>
+      <c r="B125">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>115</v>
+      </c>
+      <c r="B126">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>114</v>
+      </c>
+      <c r="B127">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>113</v>
+      </c>
+      <c r="B128">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>112</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>111</v>
+      </c>
+      <c r="B130">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>110</v>
+      </c>
+      <c r="B131">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>109</v>
+      </c>
+      <c r="B132">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>108</v>
+      </c>
+      <c r="B133">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>107</v>
+      </c>
+      <c r="B134">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>106</v>
+      </c>
+      <c r="B135">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>105</v>
+      </c>
+      <c r="B136">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>104</v>
+      </c>
+      <c r="B137">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>103</v>
+      </c>
+      <c r="B138">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>102</v>
+      </c>
+      <c r="B139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>101</v>
+      </c>
+      <c r="B140">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>100</v>
+      </c>
+      <c r="B141">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>99</v>
+      </c>
+      <c r="B142">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>98</v>
+      </c>
+      <c r="B143">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>97</v>
+      </c>
+      <c r="B144">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>96</v>
+      </c>
+      <c r="B145">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>95</v>
+      </c>
+      <c r="B146">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>94</v>
+      </c>
+      <c r="B147">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>93</v>
+      </c>
+      <c r="B148">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>92</v>
+      </c>
+      <c r="B149">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>91</v>
+      </c>
+      <c r="B150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>90</v>
+      </c>
+      <c r="B151">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>89</v>
+      </c>
+      <c r="B152">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>88</v>
+      </c>
+      <c r="B153">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>87</v>
+      </c>
+      <c r="B154">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>86</v>
+      </c>
+      <c r="B155">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>85</v>
+      </c>
+      <c r="B156">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>84</v>
+      </c>
+      <c r="B157">
+        <v>28</v>
+      </c>
+      <c r="C157" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>83</v>
+      </c>
+      <c r="B158">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>82</v>
+      </c>
+      <c r="B159">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>81</v>
+      </c>
+      <c r="B160">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>79</v>
+      </c>
+      <c r="B162">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>78</v>
+      </c>
+      <c r="B163">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>77</v>
+      </c>
+      <c r="B164">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>76</v>
+      </c>
+      <c r="B165">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>75</v>
+      </c>
+      <c r="B166">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>74</v>
+      </c>
+      <c r="B167">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>73</v>
+      </c>
+      <c r="B168">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>72</v>
+      </c>
+      <c r="B169">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>71</v>
+      </c>
+      <c r="B170">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>70</v>
+      </c>
+      <c r="B171">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>69</v>
+      </c>
+      <c r="B172">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>68</v>
+      </c>
+      <c r="B173">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>67</v>
+      </c>
+      <c r="B174">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>66</v>
+      </c>
+      <c r="B175">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>65</v>
+      </c>
+      <c r="B176">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>64</v>
+      </c>
+      <c r="B177">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>63</v>
+      </c>
+      <c r="B178">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>62</v>
+      </c>
+      <c r="B179">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>61</v>
+      </c>
+      <c r="B180">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>60</v>
+      </c>
+      <c r="B181">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>59</v>
+      </c>
+      <c r="B182">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>58</v>
+      </c>
+      <c r="B183">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>57</v>
+      </c>
+      <c r="B184">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>56</v>
+      </c>
+      <c r="B185">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>55</v>
+      </c>
+      <c r="B186">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>54</v>
+      </c>
+      <c r="B187">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>53</v>
+      </c>
+      <c r="B188">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>52</v>
+      </c>
+      <c r="B189">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>51</v>
+      </c>
+      <c r="B190">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>50</v>
+      </c>
+      <c r="B191">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>49</v>
+      </c>
+      <c r="B192">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>48</v>
+      </c>
+      <c r="B193">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>47</v>
+      </c>
+      <c r="B194">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>46</v>
+      </c>
+      <c r="B195">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>45</v>
+      </c>
+      <c r="B196">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>44</v>
+      </c>
+      <c r="B197">
+        <v>100</v>
+      </c>
+      <c r="C197" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D197" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>43</v>
+      </c>
+      <c r="B198">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>42</v>
+      </c>
+      <c r="B199">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>41</v>
+      </c>
+      <c r="B200">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>40</v>
+      </c>
+      <c r="B201">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>39</v>
+      </c>
+      <c r="B202">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>38</v>
+      </c>
+      <c r="B203">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>37</v>
+      </c>
+      <c r="B204">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>36</v>
+      </c>
+      <c r="B205">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>35</v>
+      </c>
+      <c r="B206">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>34</v>
+      </c>
+      <c r="B207">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>33</v>
+      </c>
+      <c r="B208">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>32</v>
+      </c>
+      <c r="B209">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>31</v>
+      </c>
+      <c r="B210">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>30</v>
+      </c>
+      <c r="B211">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>29</v>
+      </c>
+      <c r="B212">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>28</v>
+      </c>
+      <c r="B213">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>27</v>
+      </c>
+      <c r="B214">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>26</v>
+      </c>
+      <c r="B215">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>25</v>
+      </c>
+      <c r="B216">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>24</v>
+      </c>
+      <c r="B217">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>23</v>
+      </c>
+      <c r="B218">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>22</v>
+      </c>
+      <c r="B219">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>21</v>
+      </c>
+      <c r="B220">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>